<commit_message>
fix: upload image for csv files
</commit_message>
<xml_diff>
--- a/frontend/src/components/components/Donor Application.xlsx
+++ b/frontend/src/components/components/Donor Application.xlsx
@@ -72,10 +72,10 @@
     <t>Total Grant *</t>
   </si>
   <si>
-    <t>Years Involved*</t>
-  </si>
-  <si>
     <t>Details *</t>
+  </si>
+  <si>
+    <t>Years Involved *</t>
   </si>
 </sst>
 </file>
@@ -389,6 +389,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -408,9 +411,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,8 +632,8 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20:C20"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -652,23 +652,23 @@
     </row>
     <row r="2" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="13"/>
+      <c r="C3" s="14"/>
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="5"/>
@@ -676,7 +676,7 @@
     </row>
     <row r="5" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="5"/>
@@ -684,7 +684,7 @@
     </row>
     <row r="6" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="5"/>
@@ -692,7 +692,7 @@
     </row>
     <row r="7" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="5"/>
@@ -700,7 +700,7 @@
     </row>
     <row r="8" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="6"/>
@@ -708,7 +708,7 @@
     </row>
     <row r="9" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="5"/>
@@ -716,7 +716,7 @@
     </row>
     <row r="10" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="5"/>
@@ -724,7 +724,7 @@
     </row>
     <row r="11" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="5"/>
@@ -732,15 +732,15 @@
     </row>
     <row r="12" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="13"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="5"/>
@@ -748,7 +748,7 @@
     </row>
     <row r="14" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="5"/>
@@ -756,15 +756,15 @@
     </row>
     <row r="15" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="11"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="5"/>
@@ -772,7 +772,7 @@
     </row>
     <row r="17" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="5"/>
@@ -780,32 +780,32 @@
     </row>
     <row r="18" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="17" t="s">
-        <v>17</v>
+      <c r="B18" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="17" t="s">
-        <v>18</v>
+      <c r="B19" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="16"/>
+      <c r="C20" s="17"/>
       <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
       <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat: multiple uploads per one csv
</commit_message>
<xml_diff>
--- a/frontend/src/components/components/Donor Application.xlsx
+++ b/frontend/src/components/components/Donor Application.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>SCHOLARVISION DONOR INFORMATION</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>Years Involved *</t>
+  </si>
+  <si>
+    <t>ADDITIONAL INFORMATION</t>
+  </si>
+  <si>
+    <t>Org</t>
+  </si>
+  <si>
+    <t>Sports *</t>
   </si>
 </sst>
 </file>
@@ -629,11 +638,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -722,7 +731,7 @@
       <c r="C10" s="5"/>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="8" t="s">
         <v>12</v>
@@ -746,7 +755,7 @@
       <c r="C13" s="5"/>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="8" t="s">
         <v>14</v>
@@ -756,78 +765,103 @@
     </row>
     <row r="15" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="12"/>
+      <c r="B15" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="14"/>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="8" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="8" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="5"/>
+      <c r="B18" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="12"/>
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="1"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B21:C21"/>
+  <mergeCells count="7">
+    <mergeCell ref="B24:C24"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B23:C23"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B20:C20"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="3">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C9">
       <formula1>"M,F"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Must be a number!" sqref="C13 C17">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Must be a number!" sqref="C13 C20">
       <formula1>REGEXMATCH(TO_TEXT(C13), "^[0-9]*$")</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Must be an email!" sqref="C14">

</xml_diff>

<commit_message>
fix: data validation in Excel
</commit_message>
<xml_diff>
--- a/frontend/src/components/components/Donor Application.xlsx
+++ b/frontend/src/components/components/Donor Application.xlsx
@@ -636,7 +636,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -847,9 +847,9 @@
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B15:C15"/>
   </mergeCells>
-  <dataValidations count="3">
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C9">
-      <formula1>"M,F"</formula1>
+      <formula1>"male,female"</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Must be a number!" sqref="C13 C20">
       <formula1>REGEXMATCH(TO_TEXT(C13), "^[0-9]*$")</formula1>
@@ -857,6 +857,12 @@
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Must be an email!" sqref="C14">
       <formula1>IFERROR(ISEMAIL(C14), TRUE)</formula1>
     </dataValidation>
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
+      <formula1>1</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
+      <formula1>32874</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
fix: Uploading CSV files for Personal Statement
</commit_message>
<xml_diff>
--- a/frontend/src/components/components/Donor Application.xlsx
+++ b/frontend/src/components/components/Donor Application.xlsx
@@ -39,9 +39,6 @@
     <t>SCHOLARSHIP TO OFFER DETAILS</t>
   </si>
   <si>
-    <t>Reason/s for Applying for Personal Statement</t>
-  </si>
-  <si>
     <t>Last Name *</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>ADDITIONAL INFORMATION</t>
+  </si>
+  <si>
+    <t>Reason/s for Applying</t>
   </si>
 </sst>
 </file>
@@ -635,8 +635,8 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -672,7 +672,7 @@
     <row r="4" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="4"/>
@@ -680,7 +680,7 @@
     <row r="5" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="4"/>
@@ -704,7 +704,7 @@
     <row r="8" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="4"/>
@@ -712,7 +712,7 @@
     <row r="9" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="4"/>
@@ -720,7 +720,7 @@
     <row r="10" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="4"/>
@@ -728,7 +728,7 @@
     <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="4"/>
@@ -744,7 +744,7 @@
     <row r="13" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="4"/>
@@ -752,7 +752,7 @@
     <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="4"/>
@@ -760,7 +760,7 @@
     <row r="15" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="4"/>
@@ -788,7 +788,7 @@
     <row r="19" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="4"/>
@@ -796,7 +796,7 @@
     <row r="20" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="4"/>
@@ -804,7 +804,7 @@
     <row r="21" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="4"/>
@@ -812,7 +812,7 @@
     <row r="22" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="4"/>
@@ -820,7 +820,7 @@
     <row r="23" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="16" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C23" s="17"/>
       <c r="D23" s="4"/>
@@ -847,7 +847,7 @@
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B15:C15"/>
   </mergeCells>
-  <dataValidations count="5">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C9">
       <formula1>"male,female"</formula1>
     </dataValidation>
@@ -857,11 +857,8 @@
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Must be an email!" sqref="C14">
       <formula1>IFERROR(ISEMAIL(C14), TRUE)</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
       <formula1>1</formula1>
-    </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
-      <formula1>32874</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>